<commit_message>
update cv and add est 3 30
</commit_message>
<xml_diff>
--- a/cashflow.xlsx
+++ b/cashflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\cashflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{568FCAD8-0BCC-493E-B755-B7CA9CA09980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27030C48-A212-4F5E-B4F8-DB6440FDD38E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{DA93664B-1C47-4CFC-BC2B-8CC3DE095223}"/>
   </bookViews>
@@ -125,9 +125,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0;\(&quot;$&quot;#,##0\);&quot;-&quot;"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0;\(&quot;$&quot;#,##0\);&quot;-&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -257,7 +257,7 @@
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -265,18 +265,18 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA9CCBE-3CFF-4B4A-B418-6B7BD7E1A6DB}">
   <dimension ref="A1:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -830,88 +830,88 @@
         <v>0.9</v>
       </c>
       <c r="D3" s="3">
-        <f>MIN(1,D$2/$D$2*$C3)</f>
+        <f>MIN(1,C3*(1+(D$2/C$2-1)*$B3))</f>
         <v>0.9</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:AB3" si="4">MIN(1,E$2/$D$2*$C3)</f>
-        <v>0.86399999999999999</v>
+        <f>MIN(1,D3*(1+(E$2/D$2-1)*$B3))</f>
+        <v>0.88200000000000001</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" si="4"/>
-        <v>0.82800000000000007</v>
+        <f t="shared" ref="F3:AB3" si="4">MIN(1,E3*(1+(F$2/E$2-1)*$B3))</f>
+        <v>0.86362500000000009</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" si="4"/>
-        <v>0.79200000000000004</v>
+        <v>0.84485054347826094</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="4"/>
-        <v>0.75600000000000001</v>
+        <v>0.82564939476284593</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" si="4"/>
-        <v>0.72000000000000008</v>
+        <v>0.80599107583992102</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" si="4"/>
-        <v>0.75600000000000001</v>
+        <v>0.82614085273591897</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" si="4"/>
-        <v>0.79200000000000004</v>
+        <v>0.84581087303915503</v>
       </c>
       <c r="L3" s="3">
         <f t="shared" si="4"/>
-        <v>0.82800000000000007</v>
+        <v>0.86503384742640854</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" si="4"/>
-        <v>0.86399999999999999</v>
+        <v>0.88383893106611311</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.90225224212999056</v>
       </c>
       <c r="O3" s="3">
         <f t="shared" si="4"/>
-        <v>0.93600000000000005</v>
+        <v>0.92029728697259039</v>
       </c>
       <c r="P3" s="3">
         <f t="shared" si="4"/>
-        <v>0.97200000000000009</v>
+        <v>0.93799531172206319</v>
       </c>
       <c r="Q3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.95536559527247189</v>
       </c>
       <c r="R3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.97242569518805166</v>
       </c>
       <c r="S3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9891916554499145</v>
       </c>
       <c r="T3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99125247139876838</v>
       </c>
       <c r="U3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99331758071418241</v>
       </c>
       <c r="V3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99538699234067018</v>
       </c>
       <c r="W3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9974607152413798</v>
       </c>
       <c r="X3" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99953875839813255</v>
       </c>
       <c r="Y3" s="3">
         <f t="shared" si="4"/>
@@ -941,103 +941,103 @@
         <v>0.9</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:S5" si="5">MIN(1,D$2/$D$2*$C4)</f>
+        <f>MIN(1,C4*(1+(D$2/C$2-1)*$B4))</f>
         <v>0.9</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="5"/>
-        <v>0.86399999999999999</v>
+        <f>MIN(1,D4*(1+(E$2/D$2-1)*$B4))</f>
+        <v>0.88200000000000001</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="5"/>
-        <v>0.82800000000000007</v>
+        <f t="shared" ref="F4:AB4" si="5">MIN(1,E4*(1+(F$2/E$2-1)*$B4))</f>
+        <v>0.86362500000000009</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="5"/>
-        <v>0.79200000000000004</v>
+        <v>0.84485054347826094</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="5"/>
-        <v>0.75600000000000001</v>
+        <v>0.82564939476284593</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="5"/>
-        <v>0.72000000000000008</v>
+        <v>0.80599107583992102</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="5"/>
-        <v>0.75600000000000001</v>
+        <v>0.82614085273591897</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="5"/>
-        <v>0.79200000000000004</v>
+        <v>0.84581087303915503</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" si="5"/>
-        <v>0.82800000000000007</v>
+        <v>0.86503384742640854</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="5"/>
-        <v>0.86399999999999999</v>
+        <v>0.88383893106611311</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" si="5"/>
-        <v>0.9</v>
+        <v>0.90225224212999056</v>
       </c>
       <c r="O4" s="3">
         <f t="shared" si="5"/>
-        <v>0.93600000000000005</v>
+        <v>0.92029728697259039</v>
       </c>
       <c r="P4" s="3">
         <f t="shared" si="5"/>
-        <v>0.97200000000000009</v>
+        <v>0.93799531172206319</v>
       </c>
       <c r="Q4" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.95536559527247189</v>
       </c>
       <c r="R4" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.97242569518805166</v>
       </c>
       <c r="S4" s="3">
         <f t="shared" si="5"/>
+        <v>0.9891916554499145</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.99125247139876838</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.99331758071418241</v>
+      </c>
+      <c r="V4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.99538699234067018</v>
+      </c>
+      <c r="W4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.9974607152413798</v>
+      </c>
+      <c r="X4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.99953875839813255</v>
+      </c>
+      <c r="Y4" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="T4" s="3">
-        <f t="shared" ref="T4:AB5" si="6">MIN(1,T$2/$D$2*$C4)</f>
+      <c r="Z4" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="U4" s="3">
-        <f t="shared" si="6"/>
+      <c r="AA4" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="V4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="W4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="X4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Y4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Z4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AA4" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
       <c r="AB4" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1052,104 +1052,104 @@
         <v>0.95</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="5"/>
+        <f>MIN(1,C5*(1+(D$2/C$2-1)*$B5))</f>
         <v>0.95</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.91199999999999992</v>
+        <f>MIN(1,D5*(1+(E$2/D$2-1)*$B5))</f>
+        <v>0.9423999999999999</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.874</v>
+        <f t="shared" ref="F5:AB5" si="6">MIN(1,E5*(1+(F$2/E$2-1)*$B5))</f>
+        <v>0.93454666666666664</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.83599999999999997</v>
+        <f t="shared" si="6"/>
+        <v>0.92642017391304354</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.79799999999999993</v>
+        <f t="shared" si="6"/>
+        <v>0.91799817233201597</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.76</v>
+        <f t="shared" si="6"/>
+        <v>0.9092553325955206</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.79799999999999993</v>
+        <f t="shared" si="6"/>
+        <v>0.91834788592147587</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.83599999999999997</v>
+        <f t="shared" si="6"/>
+        <v>0.9270940562635851</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.874</v>
+        <f t="shared" si="6"/>
+        <v>0.93552218404779941</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.91199999999999992</v>
+        <f t="shared" si="6"/>
+        <v>0.94365715956125851</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.95</v>
+        <f t="shared" si="6"/>
+        <v>0.95152096922426899</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="5"/>
-        <v>0.98799999999999999</v>
+        <f t="shared" si="6"/>
+        <v>0.95913313697806313</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.96651108418558662</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.97367042554992422</v>
       </c>
       <c r="R5" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.98062521430385219</v>
       </c>
       <c r="S5" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.98738814681629261</v>
       </c>
       <c r="T5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.9882109702719728</v>
       </c>
       <c r="U5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.98903447941386602</v>
       </c>
       <c r="V5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.98985867481337753</v>
       </c>
       <c r="W5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99068355704238853</v>
       </c>
       <c r="X5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99150912667325708</v>
       </c>
       <c r="Y5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99233538427881807</v>
       </c>
       <c r="Z5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99316233043238367</v>
       </c>
       <c r="AA5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99398996570774389</v>
       </c>
       <c r="AB5" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99481829067916694</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.45">
@@ -1196,83 +1196,83 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="7"/>
-        <v>15902.676254639371</v>
+        <v>16706.261345538285</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="7"/>
-        <v>16692.942567997114</v>
+        <v>17586.848911416299</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="7"/>
-        <v>17444.521907424769</v>
+        <v>18383.097937386923</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="7"/>
-        <v>18153.396620779091</v>
+        <v>19099.299998860886</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="7"/>
-        <v>18798.64964013029</v>
+        <v>19719.214238058794</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="7"/>
-        <v>19450.080848875379</v>
+        <v>20321.451504959921</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="7"/>
-        <v>20076.15391007483</v>
+        <v>20878.595140441412</v>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="7"/>
-        <v>20641.564401272019</v>
+        <v>21359.83561852845</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="7"/>
-        <v>21223.549721479598</v>
+        <v>21870.031465554915</v>
       </c>
       <c r="R9" s="1">
         <f t="shared" si="7"/>
-        <v>21750.497236020685</v>
+        <v>22351.346319014239</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="7"/>
-        <v>22172.580013642615</v>
+        <v>22768.503177689734</v>
       </c>
       <c r="T9" s="1">
         <f t="shared" si="7"/>
-        <v>21898.231974082337</v>
+        <v>22502.797177617329</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="7"/>
-        <v>21675.313757992499</v>
+        <v>22298.533072616123</v>
       </c>
       <c r="V9" s="1">
         <f t="shared" si="7"/>
-        <v>21493.928177563434</v>
+        <v>22143.554948067958</v>
       </c>
       <c r="W9" s="1">
         <f t="shared" si="7"/>
-        <v>21355.20004755395</v>
+        <v>22037.74509031832</v>
       </c>
       <c r="X9" s="1">
         <f t="shared" si="7"/>
-        <v>21248.569840704178</v>
+        <v>21969.059624250152</v>
       </c>
       <c r="Y9" s="1">
         <f t="shared" si="7"/>
-        <v>21166.079576110464</v>
+        <v>21928.466309742049</v>
       </c>
       <c r="Z9" s="1">
         <f t="shared" si="7"/>
-        <v>21101.737528373193</v>
+        <v>21908.115911772838</v>
       </c>
       <c r="AA9" s="1">
         <f t="shared" si="7"/>
-        <v>21051.06520618996</v>
+        <v>21902.580464809569</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="7"/>
-        <v>21010.646792199288</v>
+        <v>21908.28877990627</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.45">
@@ -1284,103 +1284,103 @@
       </c>
       <c r="D10" s="1">
         <f>C10*(1+D65/12)+D53</f>
-        <v>8511</v>
+        <v>8504.9266666666663</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:AB10" si="8">D10*(1+E65/12)+E53</f>
-        <v>8633</v>
+        <v>8621.6261777777763</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="8"/>
-        <v>8755</v>
+        <v>8739.1036856296269</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="8"/>
-        <v>8838</v>
+        <v>8822.3643768671573</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="8"/>
-        <v>8921</v>
+        <v>8906.180139379605</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="8"/>
-        <v>9004</v>
+        <v>8990.5546736421347</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="8"/>
-        <v>9087</v>
+        <v>9075.4917047997478</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="8"/>
-        <v>9170</v>
+        <v>9160.9949828317458</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="8"/>
-        <v>9253</v>
+        <v>9247.0682827172895</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="8"/>
-        <v>9336</v>
+        <v>9333.7154046020714</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="8"/>
-        <v>9419</v>
+        <v>9420.9401739660843</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="8"/>
-        <v>9502</v>
+        <v>9508.7464417925239</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="8"/>
-        <v>9585</v>
+        <v>9612.9859954741278</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="8"/>
-        <v>9668</v>
+        <v>9718.0942121030785</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="8"/>
-        <v>9751</v>
+        <v>9787.0783305372697</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="8"/>
-        <v>9804</v>
+        <v>9856.6373166250796</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="8"/>
-        <v>9857</v>
+        <v>9926.7759609302884</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="8"/>
-        <v>9910</v>
+        <v>9997.4990939380405</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" si="8"/>
-        <v>9963</v>
+        <v>10068.811586387525</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="8"/>
-        <v>10016</v>
+        <v>10140.718349607419</v>
       </c>
       <c r="X10" s="1">
         <f t="shared" si="8"/>
-        <v>10069</v>
+        <v>10213.224335854147</v>
       </c>
       <c r="Y10" s="1">
         <f t="shared" si="8"/>
-        <v>10122</v>
+        <v>10286.334538652931</v>
       </c>
       <c r="Z10" s="1">
         <f t="shared" si="8"/>
-        <v>10175</v>
+        <v>10360.053993141704</v>
       </c>
       <c r="AA10" s="1">
         <f t="shared" si="8"/>
-        <v>10228</v>
+        <v>10434.387776417885</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="8"/>
-        <v>10281</v>
+        <v>10509.341007888033</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.45">
@@ -1501,103 +1501,103 @@
       </c>
       <c r="D12" s="1">
         <f>C12*(1+D$66/12)+D$49+D$55</f>
-        <v>3805.5376784817677</v>
+        <v>3867.5376784817677</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ref="E12:AB12" si="10">D12*(1+E$66/12)+E$49+E$55</f>
-        <v>4501.5695864276713</v>
+        <v>4625.6729197610048</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="10"/>
-        <v>4314.4463475074754</v>
+        <v>4500.7565197296981</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="10"/>
-        <v>4009.3899268192804</v>
+        <v>4254.0106159952065</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="10"/>
-        <v>3749.7692451290932</v>
+        <v>4052.7976354536459</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="10"/>
-        <v>2209.7062743300503</v>
+        <v>1767.6546210728957</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="10"/>
-        <v>2067.9085422953044</v>
+        <v>1632.9781383073935</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="10"/>
-        <v>1877.2039882510167</v>
+        <v>1497.4459824477342</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="10"/>
-        <v>1726.9170062830258</v>
+        <v>1439.8612691668902</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="10"/>
-        <v>1879.6233469625317</v>
+        <v>1716.5541976008094</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="10"/>
-        <v>1789.0282022820022</v>
+        <v>1771.2380710956629</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="10"/>
-        <v>1718.3663788555623</v>
+        <v>1862.3308494119256</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="10"/>
-        <v>2052.0335320742497</v>
+        <v>2369.2710807698936</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="10"/>
-        <v>1964.5998470756178</v>
+        <v>2438.7582358763657</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="10"/>
-        <v>1925.5397783271183</v>
+        <v>2564.2097259079419</v>
       </c>
       <c r="S12" s="1">
         <f t="shared" si="10"/>
-        <v>2394.6192223795742</v>
+        <v>3124.9984727158012</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" si="10"/>
-        <v>2489.7631511057302</v>
+        <v>3280.2006738881742</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="10"/>
-        <v>2532.4927127444885</v>
+        <v>3373.1125419910036</v>
       </c>
       <c r="V12" s="1">
         <f t="shared" si="10"/>
-        <v>2636.0173115175712</v>
+        <v>3519.2274650761906</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="10"/>
-        <v>2660.0786274663469</v>
+        <v>3579.5493038981549</v>
       </c>
       <c r="X12" s="1">
         <f t="shared" si="10"/>
-        <v>2651.5040885736184</v>
+        <v>3602.4064130293941</v>
       </c>
       <c r="Y12" s="1">
         <f t="shared" si="10"/>
-        <v>2775.8673891276039</v>
+        <v>3754.4596414699731</v>
       </c>
       <c r="Z12" s="1">
         <f t="shared" si="10"/>
-        <v>2671.0753271385447</v>
+        <v>3675.4835281902242</v>
       </c>
       <c r="AA12" s="1">
         <f t="shared" si="10"/>
-        <v>2552.1707942932262</v>
+        <v>3581.476043724193</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="10"/>
-        <v>2566.1813696423806</v>
+        <v>3619.6233789792723</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.45">
@@ -1609,103 +1609,103 @@
       </c>
       <c r="D13" s="18">
         <f>SUM(D9:D12)</f>
-        <v>38334.537678481771</v>
+        <v>38390.464345148437</v>
       </c>
       <c r="E13" s="18">
         <f t="shared" ref="E13:AB13" si="11">SUM(E9:E12)</f>
-        <v>37421.769586427668</v>
+        <v>37534.499097538785</v>
       </c>
       <c r="F13" s="18">
         <f t="shared" si="11"/>
-        <v>36613.679331097061</v>
+        <v>36784.093188948915</v>
       </c>
       <c r="G13" s="18">
         <f t="shared" si="11"/>
-        <v>35791.906748536479</v>
+        <v>36020.891814579561</v>
       </c>
       <c r="H13" s="18">
         <f t="shared" si="11"/>
-        <v>35016.705013695566</v>
+        <v>35304.913543399722</v>
       </c>
       <c r="I13" s="18">
         <f t="shared" si="11"/>
-        <v>34128.147598075877</v>
+        <v>34476.235709359767</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="11"/>
-        <v>34964.653677433213</v>
+        <v>35412.121321664228</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="11"/>
-        <v>35714.473216567916</v>
+        <v>36264.286223558527</v>
       </c>
       <c r="L13" s="18">
         <f t="shared" si="11"/>
-        <v>36203.439206398187</v>
+        <v>36856.355130081138</v>
       </c>
       <c r="M13" s="18">
         <f t="shared" si="11"/>
-        <v>37178.04010416993</v>
+        <v>37933.25095733878</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" si="11"/>
-        <v>37916.326529700906</v>
+        <v>38771.847228565195</v>
       </c>
       <c r="O13" s="18">
         <f t="shared" si="11"/>
-        <v>38331.620943576847</v>
+        <v>39284.773086292313</v>
       </c>
       <c r="P13" s="18">
         <f t="shared" si="11"/>
-        <v>39454.83469589585</v>
+        <v>40518.329457322048</v>
       </c>
       <c r="Q13" s="18">
         <f t="shared" si="11"/>
-        <v>40174.741494518261</v>
+        <v>41345.475839497412</v>
       </c>
       <c r="R13" s="18">
         <f t="shared" si="11"/>
-        <v>40562.037014347807</v>
+        <v>41837.634375459456</v>
       </c>
       <c r="S13" s="18">
         <f t="shared" si="11"/>
-        <v>41205.263393381356</v>
+        <v>42584.203124389787</v>
       </c>
       <c r="T13" s="18">
         <f t="shared" si="11"/>
-        <v>41191.640175475506</v>
+        <v>42656.418862723229</v>
       </c>
       <c r="U13" s="18">
         <f t="shared" si="11"/>
-        <v>41177.032413952693</v>
+        <v>42728.370651760866</v>
       </c>
       <c r="V13" s="18">
         <f t="shared" si="11"/>
-        <v>41161.567042465569</v>
+        <v>42800.215552916241</v>
       </c>
       <c r="W13" s="18">
         <f t="shared" si="11"/>
-        <v>41145.518438724612</v>
+        <v>42872.252507528217</v>
       </c>
       <c r="X13" s="18">
         <f t="shared" si="11"/>
-        <v>41128.931903301862</v>
+        <v>42944.548347157761</v>
       </c>
       <c r="Y13" s="18">
         <f t="shared" si="11"/>
-        <v>41111.886784452414</v>
+        <v>43017.2003090793</v>
       </c>
       <c r="Z13" s="18">
         <f t="shared" si="11"/>
-        <v>41094.705228334758</v>
+        <v>43090.545805927788</v>
       </c>
       <c r="AA13" s="18">
         <f t="shared" si="11"/>
-        <v>41077.080926914874</v>
+        <v>43164.289211383337</v>
       </c>
       <c r="AB13" s="18">
         <f t="shared" si="11"/>
-        <v>41059.047316597818</v>
+        <v>43238.472321529727</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.45">
@@ -1727,99 +1727,99 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" si="12"/>
-        <v>17069.916160000001</v>
+        <v>17133.086080000001</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="12"/>
-        <v>16237.593973333333</v>
+        <v>16357.408448333332</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="12"/>
-        <v>15415.800106666667</v>
+        <v>15585.81960036232</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="12"/>
-        <v>14604.53456</v>
+        <v>14818.411135461958</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="12"/>
-        <v>15012.126384379568</v>
+        <v>16058.028587461287</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="12"/>
-        <v>15878.326970678856</v>
+        <v>16975.322000456086</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="12"/>
-        <v>16718.829796075897</v>
+        <v>17816.203173026643</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="12"/>
-        <v>17528.91977702429</v>
+        <v>18583.748191321876</v>
       </c>
       <c r="M16" s="1">
         <f t="shared" si="12"/>
-        <v>18287.326369918748</v>
+        <v>19261.093237172947</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="12"/>
-        <v>19061.079231897871</v>
+        <v>19924.176240705132</v>
       </c>
       <c r="O16" s="1">
         <f t="shared" si="12"/>
-        <v>19819.179140025873</v>
+        <v>20545.779005062599</v>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="12"/>
-        <v>20525.971640624899</v>
+        <v>21094.953628689484</v>
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="12"/>
-        <v>21223.549721479598</v>
+        <v>21674.800298387447</v>
       </c>
       <c r="R16" s="1">
         <f t="shared" si="12"/>
-        <v>21750.497236020688</v>
+        <v>22228.081751742659</v>
       </c>
       <c r="S16" s="1">
         <f t="shared" si="12"/>
-        <v>22172.580013642615</v>
+        <v>22719.285212242899</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" si="12"/>
-        <v>21898.231974082337</v>
+        <v>22463.428405233546</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="12"/>
-        <v>21675.313757992499</v>
+        <v>22268.731443126147</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="12"/>
-        <v>21493.928177563434</v>
+        <v>22123.125270351913</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="12"/>
-        <v>21355.20004755395</v>
+        <v>22026.553068273883</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="12"/>
-        <v>21248.569840704182</v>
+        <v>21967.033015399633</v>
       </c>
       <c r="Y16" s="1">
         <f t="shared" si="12"/>
-        <v>21166.079576110464</v>
+        <v>21928.466309742049</v>
       </c>
       <c r="Z16" s="1">
         <f t="shared" si="12"/>
-        <v>21101.737528373193</v>
+        <v>21908.115911772838</v>
       </c>
       <c r="AA16" s="1">
         <f t="shared" si="12"/>
-        <v>21051.06520618996</v>
+        <v>21902.580464809573</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="12"/>
-        <v>21010.646792199292</v>
+        <v>21908.28877990627</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.45">
@@ -1832,103 +1832,103 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" ref="D17:AB17" si="13">D10*D3</f>
-        <v>7659.9000000000005</v>
+        <v>7654.4340000000002</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="13"/>
-        <v>7458.9120000000003</v>
+        <v>7604.2742887999984</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="13"/>
-        <v>7249.14</v>
+        <v>7547.3084205018877</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="13"/>
-        <v>6999.6959999999999</v>
+        <v>7453.579338559467</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="13"/>
-        <v>6744.2759999999998</v>
+        <v>7353.3822417276497</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="13"/>
-        <v>6482.880000000001</v>
+        <v>7246.3068338064541</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="13"/>
-        <v>6869.7719999999999</v>
+        <v>7497.634456001023</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="13"/>
-        <v>7262.64</v>
+        <v>7748.4691643362376</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="13"/>
-        <v>7661.4840000000004</v>
+        <v>7999.0270540136498</v>
       </c>
       <c r="M17" s="1">
         <f t="shared" si="13"/>
-        <v>8066.3040000000001</v>
+        <v>8249.5010460788089</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="13"/>
-        <v>8477.1</v>
+        <v>8500.0643949334026</v>
       </c>
       <c r="O17" s="1">
         <f t="shared" si="13"/>
-        <v>8893.8720000000012</v>
+        <v>8750.8735528919315</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="13"/>
-        <v>9316.6200000000008</v>
+        <v>9016.9357954045827</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="13"/>
-        <v>9668</v>
+        <v>9284.3328618598207</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" si="13"/>
-        <v>9751</v>
+        <v>9517.2064494326205</v>
       </c>
       <c r="S17" s="1">
         <f t="shared" si="13"/>
-        <v>9804</v>
+        <v>9750.1033844017657</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="13"/>
-        <v>9857</v>
+        <v>9839.941204294033</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="13"/>
-        <v>9910</v>
+        <v>9930.6916131827656</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="13"/>
-        <v>9963</v>
+        <v>10022.364081419169</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="13"/>
-        <v>10016</v>
+        <v>10114.968178060801</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="13"/>
-        <v>10069</v>
+        <v>10208.513571901247</v>
       </c>
       <c r="Y17" s="1">
         <f t="shared" si="13"/>
-        <v>10122</v>
+        <v>10286.334538652931</v>
       </c>
       <c r="Z17" s="1">
         <f t="shared" si="13"/>
-        <v>10175</v>
+        <v>10360.053993141704</v>
       </c>
       <c r="AA17" s="1">
         <f t="shared" si="13"/>
-        <v>10228</v>
+        <v>10434.387776417885</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="13"/>
-        <v>10281</v>
+        <v>10509.341007888033</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.45">
@@ -1945,99 +1945,99 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="14"/>
-        <v>6146.8799999999992</v>
+        <v>6351.7759999999989</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="14"/>
-        <v>5880.4173609906338</v>
+        <v>6287.7854042592608</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="14"/>
-        <v>5734.6117962889111</v>
+        <v>6354.8565282796226</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="14"/>
-        <v>5579.7243433160456</v>
+        <v>6418.7678562413384</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="14"/>
-        <v>5328.9414525209049</v>
+        <v>6375.4847799920417</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="14"/>
-        <v>5679.2084485783498</v>
+        <v>6535.7005920542761</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="14"/>
-        <v>6038.2167602658219</v>
+        <v>6696.1661110928289</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="14"/>
-        <v>6179.2897563397246</v>
+        <v>6614.2593234726928</v>
       </c>
       <c r="M18" s="1">
         <f t="shared" si="14"/>
-        <v>6533.3556107743225</v>
+        <v>6760.1401294593297</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="14"/>
-        <v>6895.3066046163503</v>
+        <v>6906.346130024267</v>
       </c>
       <c r="O18" s="1">
         <f t="shared" si="14"/>
-        <v>6950.6794467906911</v>
+        <v>6747.5981598474737</v>
       </c>
       <c r="P18" s="1">
         <f t="shared" si="14"/>
-        <v>7176.2367625495781</v>
+        <v>6935.9123737442569</v>
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="14"/>
-        <v>7318.5919259630491</v>
+        <v>7125.8965149786818</v>
       </c>
       <c r="R18" s="1">
         <f t="shared" si="14"/>
-        <v>7135</v>
+        <v>6996.7609040579855</v>
       </c>
       <c r="S18" s="1">
         <f t="shared" si="14"/>
-        <v>6834.0641573591693</v>
+        <v>6747.8739435585185</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="14"/>
-        <v>6946.6450502874359</v>
+        <v>6864.7508452795446</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="14"/>
-        <v>7059.2259432157025</v>
+        <v>6981.8178558131995</v>
       </c>
       <c r="V18" s="1">
         <f t="shared" si="14"/>
-        <v>7068.6215533845652</v>
+        <v>6996.9363635905238</v>
       </c>
       <c r="W18" s="1">
         <f t="shared" si="14"/>
-        <v>7114.239763704315</v>
+        <v>7047.9603547589923</v>
       </c>
       <c r="X18" s="1">
         <f t="shared" si="14"/>
-        <v>7159.8579740240648</v>
+        <v>7099.0645269291563</v>
       </c>
       <c r="Y18" s="1">
         <f t="shared" si="14"/>
-        <v>7047.9398192143481</v>
+        <v>6993.9200688740539</v>
       </c>
       <c r="Z18" s="1">
         <f t="shared" si="14"/>
-        <v>7146.8923728230175</v>
+        <v>7098.0242843423366</v>
       </c>
       <c r="AA18" s="1">
         <f t="shared" si="14"/>
-        <v>7245.8449264316869</v>
+        <v>7202.2971499474625</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="14"/>
-        <v>7201.2191547561524</v>
+        <v>7163.904530340591</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.45">
@@ -2050,103 +2050,103 @@
       </c>
       <c r="D19" s="1">
         <f>D12</f>
-        <v>3805.5376784817677</v>
+        <v>3867.5376784817677</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" ref="E19:AB19" si="15">D19*(1+E66/12)+E49+E55</f>
-        <v>4501.5695864276713</v>
+        <v>4625.6729197610048</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="15"/>
-        <v>4314.4463475074754</v>
+        <v>4500.7565197296981</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="15"/>
-        <v>4009.3899268192804</v>
+        <v>4254.0106159952065</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="15"/>
-        <v>3749.7692451290932</v>
+        <v>4052.7976354536459</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="15"/>
-        <v>2209.7062743300503</v>
+        <v>1767.6546210728957</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="15"/>
-        <v>2067.9085422953044</v>
+        <v>1632.9781383073935</v>
       </c>
       <c r="K19" s="1">
         <f t="shared" si="15"/>
-        <v>1877.2039882510167</v>
+        <v>1497.4459824477342</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="15"/>
-        <v>1726.9170062830258</v>
+        <v>1439.8612691668902</v>
       </c>
       <c r="M19" s="1">
         <f t="shared" si="15"/>
-        <v>1879.6233469625317</v>
+        <v>1716.5541976008094</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="15"/>
-        <v>1789.0282022820022</v>
+        <v>1771.2380710956629</v>
       </c>
       <c r="O19" s="1">
         <f t="shared" si="15"/>
-        <v>1718.3663788555623</v>
+        <v>1862.3308494119256</v>
       </c>
       <c r="P19" s="1">
         <f t="shared" si="15"/>
-        <v>2052.0335320742497</v>
+        <v>2369.2710807698936</v>
       </c>
       <c r="Q19" s="1">
         <f t="shared" si="15"/>
-        <v>1964.5998470756178</v>
+        <v>2438.7582358763657</v>
       </c>
       <c r="R19" s="1">
         <f t="shared" si="15"/>
-        <v>1925.5397783271183</v>
+        <v>2564.2097259079419</v>
       </c>
       <c r="S19" s="1">
         <f t="shared" si="15"/>
-        <v>2394.6192223795742</v>
+        <v>3124.9984727158012</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="15"/>
-        <v>2489.7631511057302</v>
+        <v>3280.2006738881742</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="15"/>
-        <v>2532.4927127444885</v>
+        <v>3373.1125419910036</v>
       </c>
       <c r="V19" s="1">
         <f t="shared" si="15"/>
-        <v>2636.0173115175712</v>
+        <v>3519.2274650761906</v>
       </c>
       <c r="W19" s="1">
         <f t="shared" si="15"/>
-        <v>2660.0786274663469</v>
+        <v>3579.5493038981549</v>
       </c>
       <c r="X19" s="1">
         <f t="shared" si="15"/>
-        <v>2651.5040885736184</v>
+        <v>3602.4064130293941</v>
       </c>
       <c r="Y19" s="1">
         <f t="shared" si="15"/>
-        <v>2775.8673891276039</v>
+        <v>3754.4596414699731</v>
       </c>
       <c r="Z19" s="1">
         <f t="shared" si="15"/>
-        <v>2671.0753271385447</v>
+        <v>3675.4835281902242</v>
       </c>
       <c r="AA19" s="1">
         <f t="shared" si="15"/>
-        <v>2552.1707942932262</v>
+        <v>3581.476043724193</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="15"/>
-        <v>2566.1813696423806</v>
+        <v>3619.6233789792723</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.45">
@@ -2159,103 +2159,103 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" ref="D20:AB20" si="16">SUM(D16:D19)</f>
-        <v>36762.137678481769</v>
+        <v>36818.671678481769</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="16"/>
-        <v>35177.277746427673</v>
+        <v>35714.809288561002</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="16"/>
-        <v>33681.597681831438</v>
+        <v>34693.258792824177</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="16"/>
-        <v>32159.497829774857</v>
+        <v>33648.266083196613</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="16"/>
-        <v>30678.304148445139</v>
+        <v>32643.358868884592</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="16"/>
-        <v>29033.65411123052</v>
+        <v>31447.474822332679</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="16"/>
-        <v>30495.215961552509</v>
+        <v>32641.635186818778</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="16"/>
-        <v>31896.890544592738</v>
+        <v>33758.284430903441</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="16"/>
-        <v>33096.610539647038</v>
+        <v>34636.895837975113</v>
       </c>
       <c r="M20" s="1">
         <f t="shared" si="16"/>
-        <v>34766.609327655598</v>
+        <v>35987.288610311894</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="16"/>
-        <v>36222.514038796224</v>
+        <v>37101.82483675846</v>
       </c>
       <c r="O20" s="1">
         <f t="shared" si="16"/>
-        <v>37382.096965672135</v>
+        <v>37906.581567213929</v>
       </c>
       <c r="P20" s="1">
         <f t="shared" si="16"/>
-        <v>39070.861935248729</v>
+        <v>39417.072878608218</v>
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="16"/>
-        <v>40174.741494518261</v>
+        <v>40523.787911102314</v>
       </c>
       <c r="R20" s="1">
         <f t="shared" si="16"/>
-        <v>40562.037014347807</v>
+        <v>41306.258831141211</v>
       </c>
       <c r="S20" s="1">
         <f t="shared" si="16"/>
-        <v>41205.263393381356</v>
+        <v>42342.261012918985</v>
       </c>
       <c r="T20" s="1">
         <f t="shared" si="16"/>
-        <v>41191.640175475506</v>
+        <v>42448.321128695301</v>
       </c>
       <c r="U20" s="1">
         <f t="shared" si="16"/>
-        <v>41177.032413952693</v>
+        <v>42554.353454113116</v>
       </c>
       <c r="V20" s="1">
         <f t="shared" si="16"/>
-        <v>41161.567042465569</v>
+        <v>42661.653180437796</v>
       </c>
       <c r="W20" s="1">
         <f t="shared" si="16"/>
-        <v>41145.518438724612</v>
+        <v>42769.030904991829</v>
       </c>
       <c r="X20" s="1">
         <f t="shared" si="16"/>
-        <v>41128.931903301862</v>
+        <v>42877.017527259428</v>
       </c>
       <c r="Y20" s="1">
         <f t="shared" si="16"/>
-        <v>41111.886784452414</v>
+        <v>42963.180558739004</v>
       </c>
       <c r="Z20" s="1">
         <f t="shared" si="16"/>
-        <v>41094.705228334758</v>
+        <v>43041.677717447106</v>
       </c>
       <c r="AA20" s="1">
         <f t="shared" si="16"/>
-        <v>41077.080926914874</v>
+        <v>43120.741434899115</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="16"/>
-        <v>41059.047316597818</v>
+        <v>43201.157697114169</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.45">
@@ -2399,103 +2399,103 @@
       <c r="C23" s="1"/>
       <c r="D23" s="8">
         <f>D20/(C20+D49)-1</f>
-        <v>-2.0390317278904391E-3</v>
+        <v>-5.0433519109682745E-4</v>
       </c>
       <c r="E23" s="8">
         <f t="shared" ref="E23:AB23" si="18">E20/(D20+E49)-1</f>
-        <v>-4.0239397357714757E-2</v>
+        <v>-2.7074321801280443E-2</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="18"/>
-        <v>-3.951490259997148E-2</v>
+        <v>-2.5601892383388947E-2</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" si="18"/>
-        <v>-4.2062336902744191E-2</v>
+        <v>-2.7035992045421953E-2</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="18"/>
-        <v>-4.2783624523933805E-2</v>
+        <v>-2.6683168774798038E-2</v>
       </c>
       <c r="I23" s="8">
         <f t="shared" si="18"/>
-        <v>-5.0203963875852686E-2</v>
+        <v>-3.3377557199925967E-2</v>
       </c>
       <c r="J23" s="8">
         <f t="shared" si="18"/>
-        <v>5.4334830733291817E-2</v>
+        <v>4.1616638605376233E-2</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="18"/>
-        <v>4.9750332034927958E-2</v>
+        <v>3.7706350665756894E-2</v>
       </c>
       <c r="L23" s="8">
         <f t="shared" si="18"/>
-        <v>4.1203149242199144E-2</v>
+        <v>2.9380737347896035E-2</v>
       </c>
       <c r="M23" s="8">
         <f t="shared" si="18"/>
-        <v>5.396125151655573E-2</v>
+        <v>4.2297250792251662E-2</v>
       </c>
       <c r="N23" s="8">
         <f t="shared" si="18"/>
-        <v>4.5183436623474016E-2</v>
+        <v>3.413123660896189E-2</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" si="18"/>
-        <v>3.5156315218374923E-2</v>
+        <v>2.4728618674320746E-2</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="18"/>
-        <v>4.826036407968326E-2</v>
+        <v>4.2874017813292475E-2</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="18"/>
-        <v>3.1156383585325909E-2</v>
+        <v>3.0954099183413408E-2</v>
       </c>
       <c r="R23" s="8">
         <f t="shared" si="18"/>
-        <v>1.2412298227297613E-2</v>
+        <v>2.2083327650505247E-2</v>
       </c>
       <c r="S23" s="8">
         <f t="shared" si="18"/>
-        <v>1.862023360569931E-2</v>
+        <v>2.7818112962031405E-2</v>
       </c>
       <c r="T23" s="8">
         <f t="shared" si="18"/>
-        <v>2.3452041460736428E-3</v>
+        <v>5.1159968847092063E-3</v>
       </c>
       <c r="U23" s="8">
         <f t="shared" si="18"/>
-        <v>2.3220163087387391E-3</v>
+        <v>5.1025246079348108E-3</v>
       </c>
       <c r="V23" s="8">
         <f t="shared" si="18"/>
-        <v>2.3019590887398689E-3</v>
+        <v>5.1196380352360737E-3</v>
       </c>
       <c r="W23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2886189986817129E-3</v>
+        <v>5.1085612028340943E-3</v>
       </c>
       <c r="X23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2764051273469477E-3</v>
+        <v>5.1099759568633552E-3</v>
       </c>
       <c r="Y23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2661458218775632E-3</v>
+        <v>4.5867830590371472E-3</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2637603086486102E-3</v>
+        <v>4.39867370987157E-3</v>
       </c>
       <c r="AA23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2539066235922611E-3</v>
+        <v>4.4038278377174223E-3</v>
       </c>
       <c r="AB23" s="8">
         <f t="shared" si="18"/>
-        <v>2.2448851029199801E-3</v>
+        <v>4.4271792548209454E-3</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.45">
@@ -2513,103 +2513,103 @@
       </c>
       <c r="D26" s="8">
         <f t="shared" ref="D26:AB26" si="19">D16/D$20</f>
-        <v>0.51502989748832073</v>
+        <v>0.51423908405325536</v>
       </c>
       <c r="E26" s="8">
         <f t="shared" si="19"/>
-        <v>0.48525404049304205</v>
+        <v>0.47971937751568816</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="19"/>
-        <v>0.48209096631102605</v>
+        <v>0.47148665237860665</v>
       </c>
       <c r="G26" s="8">
         <f t="shared" si="19"/>
-        <v>0.47935450324084217</v>
+        <v>0.4631982985936271</v>
       </c>
       <c r="H26" s="8">
         <f t="shared" si="19"/>
-        <v>0.47605416809651774</v>
+        <v>0.45394872491466426</v>
       </c>
       <c r="I26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51705948988944939</v>
+        <v>0.51063014369781923</v>
       </c>
       <c r="J26" s="8">
         <f t="shared" si="19"/>
-        <v>0.5206825552800739</v>
+        <v>0.52005121383474673</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52415233932293526</v>
+        <v>0.52775795551734572</v>
       </c>
       <c r="L26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52962884993996817</v>
+        <v>0.53653041768676835</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52600258476663786</v>
+        <v>0.53521935052516911</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52622187437024526</v>
+        <v>0.53701337679125005</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" si="19"/>
-        <v>0.53017836742079405</v>
+        <v>0.54201086343362093</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52535241415052825</v>
+        <v>0.53517301230497483</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52828092806460236</v>
+        <v>0.5348660975606675</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="19"/>
-        <v>0.53622793224923571</v>
+        <v>0.53812866090367595</v>
       </c>
       <c r="S26" s="8">
         <f t="shared" si="19"/>
-        <v>0.53810067422610175</v>
+        <v>0.53656287285440551</v>
       </c>
       <c r="T26" s="8">
         <f t="shared" si="19"/>
-        <v>0.53161835461749851</v>
+        <v>0.52919474334753236</v>
       </c>
       <c r="U26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52639329469133611</v>
+        <v>0.52330089956927195</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="19"/>
-        <v>0.52218439971900432</v>
+        <v>0.51857168255486918</v>
       </c>
       <c r="W26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51901642895463529</v>
+        <v>0.51501174102364411</v>
       </c>
       <c r="X26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51663315475008309</v>
+        <v>0.51232651621428438</v>
       </c>
       <c r="Y26" s="8">
         <f t="shared" si="19"/>
-        <v>0.5148408704052716</v>
+        <v>0.51040137216474424</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51349042196860839</v>
+        <v>0.5089977220588755</v>
       </c>
       <c r="AA26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51247714616441264</v>
+        <v>0.50793608217234998</v>
       </c>
       <c r="AB26" s="8">
         <f t="shared" si="19"/>
-        <v>0.51171783480972033</v>
+        <v>0.50712272419888738</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.45">
@@ -2622,103 +2622,103 @@
       </c>
       <c r="D27" s="8">
         <f t="shared" ref="D27:AB27" si="20">D17/D$20</f>
-        <v>0.20836383528598831</v>
+        <v>0.20789544139023197</v>
       </c>
       <c r="E27" s="8">
         <f t="shared" si="20"/>
-        <v>0.21203778341709426</v>
+        <v>0.21291655871267806</v>
       </c>
       <c r="F27" s="8">
         <f t="shared" si="20"/>
-        <v>0.21522553854119394</v>
+        <v>0.21754394608969235</v>
       </c>
       <c r="G27" s="8">
         <f t="shared" si="20"/>
-        <v>0.21765563744342223</v>
+        <v>0.22151451489744553</v>
       </c>
       <c r="H27" s="8">
         <f t="shared" si="20"/>
-        <v>0.2198386184375129</v>
+        <v>0.22526426496927801</v>
       </c>
       <c r="I27" s="8">
         <f t="shared" si="20"/>
-        <v>0.22328846293902618</v>
+        <v>0.23042571382108018</v>
       </c>
       <c r="J27" s="8">
         <f t="shared" si="20"/>
-        <v>0.22527376125688733</v>
+        <v>0.22969543079228733</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="20"/>
-        <v>0.22769115973378748</v>
+        <v>0.22952793054978335</v>
       </c>
       <c r="L27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23148847797638275</v>
+        <v>0.23093948982702128</v>
       </c>
       <c r="M27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23201296174670513</v>
+        <v>0.22923374793273463</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23402848269782101</v>
+        <v>0.229100979057828</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23791795329639256</v>
+        <v>0.230853672135414</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23845442712372786</v>
+        <v>0.22875711301987889</v>
       </c>
       <c r="Q27" s="8">
         <f t="shared" si="20"/>
-        <v>0.2406487170880533</v>
+        <v>0.22910821866472628</v>
       </c>
       <c r="R27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24039719692950401</v>
+        <v>0.2304059171356739</v>
       </c>
       <c r="S27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23793076885354358</v>
+        <v>0.23026884136931011</v>
       </c>
       <c r="T27" s="8">
         <f t="shared" si="20"/>
-        <v>0.23929612800095823</v>
+        <v>0.23180990302210511</v>
       </c>
       <c r="U27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24066814481371007</v>
+        <v>0.2333648806083061</v>
       </c>
       <c r="V27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24204617841010209</v>
+        <v>0.23492676289475942</v>
       </c>
       <c r="W27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24342869843567988</v>
+        <v>0.23650215971763397</v>
       </c>
       <c r="X27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24481549931014993</v>
+        <v>0.23808823842309224</v>
       </c>
       <c r="Y27" s="8">
         <f t="shared" si="20"/>
-        <v>0.2462061654593754</v>
+        <v>0.23942209130884795</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24759880727856753</v>
+        <v>0.24069819167253831</v>
       </c>
       <c r="AA27" s="8">
         <f t="shared" si="20"/>
-        <v>0.24899529784499178</v>
+        <v>0.24198071343859065</v>
       </c>
       <c r="AB27" s="8">
         <f t="shared" si="20"/>
-        <v>0.25039548338093032</v>
+        <v>0.24326526343505966</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.45">
@@ -2731,103 +2731,103 @@
       </c>
       <c r="D28" s="8">
         <f t="shared" ref="D28:AB28" si="21">D18/D$20</f>
-        <v>0.17308841111610754</v>
+        <v>0.17282263889272348</v>
       </c>
       <c r="E28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17474007068736944</v>
+        <v>0.17784712074703396</v>
       </c>
       <c r="F28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17458843302325455</v>
+        <v>0.18123939990208709</v>
       </c>
       <c r="G28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17831782780449773</v>
+        <v>0.18886133723999327</v>
       </c>
       <c r="H28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18187851311197203</v>
+        <v>0.19663319213022715</v>
       </c>
       <c r="I28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18354360192159261</v>
+        <v>0.20273439492395873</v>
       </c>
       <c r="J28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18623276699330585</v>
+        <v>0.20022589415782388</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18930424430632908</v>
+        <v>0.1983562323730805</v>
       </c>
       <c r="L28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18670460979493475</v>
+        <v>0.19095993343089851</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" si="21"/>
-        <v>0.1879204137855707</v>
+        <v>0.18784799829354915</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" si="21"/>
-        <v>0.19035969168874123</v>
+        <v>0.18614572626578293</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18593604990039694</v>
+        <v>0.17800597893225989</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18367234320150386</v>
+        <v>0.1759621368919152</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="21"/>
-        <v>0.18216898612680935</v>
+        <v>0.17584477864238349</v>
       </c>
       <c r="R28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17590339453307466</v>
+        <v>0.16938742704006532</v>
       </c>
       <c r="S28" s="8">
         <f t="shared" si="21"/>
-        <v>0.16585415538095793</v>
+        <v>0.15936498859849937</v>
       </c>
       <c r="T28" s="8">
         <f t="shared" si="21"/>
-        <v>0.1686421084641174</v>
+        <v>0.16172019676507146</v>
       </c>
       <c r="U28" s="8">
         <f t="shared" si="21"/>
-        <v>0.1714360052042922</v>
+        <v>0.16406823953609775</v>
       </c>
       <c r="V28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17172867947646428</v>
+        <v>0.16400996778059507</v>
       </c>
       <c r="W28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17290436561879996</v>
+        <v>0.16479121003268707</v>
       </c>
       <c r="X28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17408324609201112</v>
+        <v>0.1655680580491837</v>
       </c>
       <c r="Y28" s="8">
         <f t="shared" si="21"/>
-        <v>0.1714331394267149</v>
+        <v>0.16278869436381713</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17391272995177107</v>
+        <v>0.16491049282368297</v>
       </c>
       <c r="AA28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17639629601050844</v>
+        <v>0.16702628271874734</v>
       </c>
       <c r="AB28" s="8">
         <f t="shared" si="21"/>
-        <v>0.17538690314047087</v>
+        <v>0.16582667947389609</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.45">
@@ -2840,103 +2840,103 @@
       </c>
       <c r="D29" s="8">
         <f t="shared" ref="D29:AB29" si="22">D19/D$20</f>
-        <v>0.10351785610958333</v>
+        <v>0.10504283566378914</v>
       </c>
       <c r="E29" s="8">
         <f t="shared" si="22"/>
-        <v>0.12796810540249423</v>
+        <v>0.12951694302459985</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" si="22"/>
-        <v>0.12809506212452559</v>
+        <v>0.12973000162961393</v>
       </c>
       <c r="G29" s="8">
         <f t="shared" si="22"/>
-        <v>0.12467203151123799</v>
+        <v>0.12642584926893422</v>
       </c>
       <c r="H29" s="8">
         <f t="shared" si="22"/>
-        <v>0.1222287003539973</v>
+        <v>0.12415381798583057</v>
       </c>
       <c r="I29" s="8">
         <f t="shared" si="22"/>
-        <v>7.6108445249931975E-2</v>
+        <v>5.6209747557141899E-2</v>
       </c>
       <c r="J29" s="8">
         <f t="shared" si="22"/>
-        <v>6.781091646973296E-2</v>
+        <v>5.002746121514208E-2</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="22"/>
-        <v>5.8852256636948153E-2</v>
+        <v>4.4357881559790494E-2</v>
       </c>
       <c r="L29" s="8">
         <f t="shared" si="22"/>
-        <v>5.2178062288714432E-2</v>
+        <v>4.157015905531173E-2</v>
       </c>
       <c r="M29" s="8">
         <f t="shared" si="22"/>
-        <v>5.4064039701086364E-2</v>
+        <v>4.7698903248547135E-2</v>
       </c>
       <c r="N29" s="8">
         <f t="shared" si="22"/>
-        <v>4.9389951243192523E-2</v>
+        <v>4.7739917885139087E-2</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" si="22"/>
-        <v>4.5967629382416213E-2</v>
+        <v>4.9129485498705279E-2</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="22"/>
-        <v>5.2520815524240011E-2</v>
+        <v>6.0107737783231113E-2</v>
       </c>
       <c r="Q29" s="8">
         <f t="shared" si="22"/>
-        <v>4.8901368720535077E-2</v>
+        <v>6.0180905132222802E-2</v>
       </c>
       <c r="R29" s="8">
         <f t="shared" si="22"/>
-        <v>4.7471476288185592E-2</v>
+        <v>6.2077994920584724E-2</v>
       </c>
       <c r="S29" s="8">
         <f t="shared" si="22"/>
-        <v>5.811440153939685E-2</v>
+        <v>7.3803297177785041E-2</v>
       </c>
       <c r="T29" s="8">
         <f t="shared" si="22"/>
-        <v>6.0443408917425778E-2</v>
+        <v>7.7275156865290962E-2</v>
       </c>
       <c r="U29" s="8">
         <f t="shared" si="22"/>
-        <v>6.1502555290661551E-2</v>
+        <v>7.9265980286324228E-2</v>
       </c>
       <c r="V29" s="8">
         <f t="shared" si="22"/>
-        <v>6.4040742394429362E-2</v>
+        <v>8.2491586769776373E-2</v>
       </c>
       <c r="W29" s="8">
         <f t="shared" si="22"/>
-        <v>6.4650506990884843E-2</v>
+        <v>8.3694889226034921E-2</v>
       </c>
       <c r="X29" s="8">
         <f t="shared" si="22"/>
-        <v>6.4468099847755922E-2</v>
+        <v>8.401718731343974E-2</v>
       </c>
       <c r="Y29" s="8">
         <f t="shared" si="22"/>
-        <v>6.751982470863814E-2</v>
+        <v>8.7387842162590781E-2</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="22"/>
-        <v>6.4998040801052898E-2</v>
+        <v>8.5393593444903132E-2</v>
       </c>
       <c r="AA29" s="8">
         <f t="shared" si="22"/>
-        <v>6.2131259980087124E-2</v>
+        <v>8.3056921670312006E-2</v>
       </c>
       <c r="AB29" s="8">
         <f t="shared" si="22"/>
-        <v>6.2499778668878674E-2</v>
+        <v>8.3785332892156783E-2</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.45">
@@ -3369,103 +3369,103 @@
       </c>
       <c r="D38" s="9">
         <f t="shared" ref="D38:AB41" si="27">D26-D32</f>
-        <v>-8.3034358450125856E-3</v>
+        <v>-9.0942492800779595E-3</v>
       </c>
       <c r="E38" s="9">
         <f t="shared" si="27"/>
-        <v>-3.6690403951402384E-2</v>
+        <v>-4.2225066928756272E-2</v>
       </c>
       <c r="F38" s="9">
         <f t="shared" si="27"/>
-        <v>-3.8464589244529501E-2</v>
+        <v>-4.9068903176948897E-2</v>
       </c>
       <c r="G38" s="9">
         <f t="shared" si="27"/>
-        <v>-3.9812163425824498E-2</v>
+        <v>-5.5968368073039565E-2</v>
       </c>
       <c r="H38" s="9">
         <f t="shared" si="27"/>
-        <v>-4.1723609681260043E-2</v>
+        <v>-6.3829052863113522E-2</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" si="27"/>
-        <v>6.7060100056048899E-4</v>
+        <v>-5.7587451910696696E-3</v>
       </c>
       <c r="J38" s="9">
         <f t="shared" si="27"/>
-        <v>5.6825552800738865E-3</v>
+        <v>5.051213834746715E-3</v>
       </c>
       <c r="K38" s="9">
         <f t="shared" si="27"/>
-        <v>1.0541228211824238E-2</v>
+        <v>1.4146844406234704E-2</v>
       </c>
       <c r="L38" s="9">
         <f t="shared" si="27"/>
-        <v>1.7406627717746037E-2</v>
+        <v>2.4308195464546212E-2</v>
       </c>
       <c r="M38" s="9">
         <f t="shared" si="27"/>
-        <v>1.5169251433304609E-2</v>
+        <v>2.4386017191835863E-2</v>
       </c>
       <c r="N38" s="9">
         <f t="shared" si="27"/>
-        <v>1.6777429925800891E-2</v>
+        <v>2.7568932346805686E-2</v>
       </c>
       <c r="O38" s="9">
         <f t="shared" si="27"/>
-        <v>2.2122811865238567E-2</v>
+        <v>3.3955307878065444E-2</v>
       </c>
       <c r="P38" s="9">
         <f t="shared" si="27"/>
-        <v>1.8685747483861648E-2</v>
+        <v>2.8506345638308228E-2</v>
       </c>
       <c r="Q38" s="9">
         <f t="shared" si="27"/>
-        <v>2.3003150286824647E-2</v>
+        <v>2.9588319782889783E-2</v>
       </c>
       <c r="R38" s="9">
         <f t="shared" si="27"/>
-        <v>3.2339043360346875E-2</v>
+        <v>3.4239772014787118E-2</v>
       </c>
       <c r="S38" s="9">
         <f t="shared" si="27"/>
-        <v>3.5600674226101914E-2</v>
+        <v>3.4062872854405679E-2</v>
       </c>
       <c r="T38" s="9">
         <f t="shared" si="27"/>
-        <v>3.050724350638756E-2</v>
+        <v>2.8083632236421407E-2</v>
       </c>
       <c r="U38" s="9">
         <f t="shared" si="27"/>
-        <v>2.6393294691336111E-2</v>
+        <v>2.3300899569271949E-2</v>
       </c>
       <c r="V38" s="9">
         <f t="shared" si="27"/>
-        <v>2.2184399719004322E-2</v>
+        <v>1.8571682554869184E-2</v>
       </c>
       <c r="W38" s="9">
         <f t="shared" si="27"/>
-        <v>1.9016428954635289E-2</v>
+        <v>1.501174102364411E-2</v>
       </c>
       <c r="X38" s="9">
         <f t="shared" si="27"/>
-        <v>1.663315475008309E-2</v>
+        <v>1.2326516214284378E-2</v>
       </c>
       <c r="Y38" s="9">
         <f t="shared" si="27"/>
-        <v>1.48408704052716E-2</v>
+        <v>1.0401372164744238E-2</v>
       </c>
       <c r="Z38" s="9">
         <f t="shared" si="27"/>
-        <v>1.349042196860839E-2</v>
+        <v>8.9977220588755014E-3</v>
       </c>
       <c r="AA38" s="9">
         <f t="shared" si="27"/>
-        <v>1.2477146164412645E-2</v>
+        <v>7.9360821723499786E-3</v>
       </c>
       <c r="AB38" s="9">
         <f t="shared" si="27"/>
-        <v>1.1717834809720329E-2</v>
+        <v>7.1227241988873757E-3</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.45">
@@ -3478,103 +3478,103 @@
       </c>
       <c r="D39" s="9">
         <f t="shared" si="28"/>
-        <v>8.3638352859883025E-3</v>
+        <v>7.8954413902319609E-3</v>
       </c>
       <c r="E39" s="9">
         <f t="shared" si="28"/>
-        <v>1.2037783417094244E-2</v>
+        <v>1.291655871267805E-2</v>
       </c>
       <c r="F39" s="9">
         <f t="shared" si="28"/>
-        <v>1.5225538541193934E-2</v>
+        <v>1.7543946089692342E-2</v>
       </c>
       <c r="G39" s="9">
         <f t="shared" si="28"/>
-        <v>1.7655637443422217E-2</v>
+        <v>2.1514514897445519E-2</v>
       </c>
       <c r="H39" s="9">
         <f t="shared" si="28"/>
-        <v>1.9838618437512889E-2</v>
+        <v>2.5264264969278E-2</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="28"/>
-        <v>2.3288462939026172E-2</v>
+        <v>3.0425713821080169E-2</v>
       </c>
       <c r="J39" s="9">
         <f t="shared" si="28"/>
-        <v>2.5273761256887323E-2</v>
+        <v>2.9695430792287314E-2</v>
       </c>
       <c r="K39" s="9">
         <f t="shared" si="28"/>
-        <v>2.7691159733787468E-2</v>
+        <v>2.9527930549783338E-2</v>
       </c>
       <c r="L39" s="9">
         <f t="shared" si="28"/>
-        <v>3.1488477976382739E-2</v>
+        <v>3.0939489827021271E-2</v>
       </c>
       <c r="M39" s="9">
         <f t="shared" si="28"/>
-        <v>3.2012961746705121E-2</v>
+        <v>2.9233747932734616E-2</v>
       </c>
       <c r="N39" s="9">
         <f t="shared" si="28"/>
-        <v>3.4028482697820994E-2</v>
+        <v>2.9100979057827991E-2</v>
       </c>
       <c r="O39" s="9">
         <f t="shared" si="28"/>
-        <v>3.7917953296392554E-2</v>
+        <v>3.0853672135413984E-2</v>
       </c>
       <c r="P39" s="9">
         <f t="shared" si="28"/>
-        <v>3.8454427123727847E-2</v>
+        <v>2.8757113019878877E-2</v>
       </c>
       <c r="Q39" s="9">
         <f t="shared" si="28"/>
-        <v>4.0648717088053288E-2</v>
+        <v>2.9108218664726265E-2</v>
       </c>
       <c r="R39" s="9">
         <f t="shared" si="28"/>
-        <v>4.0397196929503998E-2</v>
+        <v>3.0405917135673893E-2</v>
       </c>
       <c r="S39" s="9">
         <f t="shared" si="27"/>
-        <v>3.7930768853543573E-2</v>
+        <v>3.0268841369310101E-2</v>
       </c>
       <c r="T39" s="9">
         <f t="shared" si="27"/>
-        <v>3.9296128000958219E-2</v>
+        <v>3.1809903022105096E-2</v>
       </c>
       <c r="U39" s="9">
         <f t="shared" si="27"/>
-        <v>4.0668144813710061E-2</v>
+        <v>3.3364880608306086E-2</v>
       </c>
       <c r="V39" s="9">
         <f t="shared" si="27"/>
-        <v>4.2046178410102081E-2</v>
+        <v>3.4926762894759406E-2</v>
       </c>
       <c r="W39" s="9">
         <f t="shared" si="27"/>
-        <v>4.3428698435679869E-2</v>
+        <v>3.6502159717633959E-2</v>
       </c>
       <c r="X39" s="9">
         <f t="shared" si="27"/>
-        <v>4.4815499310149914E-2</v>
+        <v>3.8088238423092224E-2</v>
       </c>
       <c r="Y39" s="9">
         <f t="shared" si="27"/>
-        <v>4.6206165459375392E-2</v>
+        <v>3.942209130884794E-2</v>
       </c>
       <c r="Z39" s="9">
         <f t="shared" si="27"/>
-        <v>4.7598807278567523E-2</v>
+        <v>4.0698191672538298E-2</v>
       </c>
       <c r="AA39" s="9">
         <f t="shared" si="27"/>
-        <v>4.8995297844991764E-2</v>
+        <v>4.1980713438590639E-2</v>
       </c>
       <c r="AB39" s="9">
         <f t="shared" si="27"/>
-        <v>5.0395483380930306E-2</v>
+        <v>4.3265263435059653E-2</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.45">
@@ -3587,103 +3587,103 @@
       </c>
       <c r="D40" s="9">
         <f t="shared" si="27"/>
-        <v>1.0884111161075516E-3</v>
+        <v>8.2263889272349289E-4</v>
       </c>
       <c r="E40" s="9">
         <f t="shared" si="27"/>
-        <v>1.0734040207027729E-3</v>
+        <v>4.1804540803672963E-3</v>
       </c>
       <c r="F40" s="9">
         <f t="shared" si="27"/>
-        <v>-7.4490031007878876E-4</v>
+        <v>5.9060665687537539E-3</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="27"/>
-        <v>1.3178278044977121E-3</v>
+        <v>1.1861337239993247E-2</v>
       </c>
       <c r="H40" s="9">
         <f t="shared" si="27"/>
-        <v>3.2118464453053386E-3</v>
+        <v>1.7966525463560451E-2</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" si="27"/>
-        <v>3.2102685882592352E-3</v>
+        <v>2.2401061590625354E-2</v>
       </c>
       <c r="J40" s="9">
         <f t="shared" si="27"/>
-        <v>4.2327669933057976E-3</v>
+        <v>1.822589415782383E-2</v>
       </c>
       <c r="K40" s="9">
         <f t="shared" si="27"/>
-        <v>5.6375776396623556E-3</v>
+        <v>1.4689565706413776E-2</v>
       </c>
       <c r="L40" s="9">
         <f t="shared" si="27"/>
-        <v>1.3712764616013451E-3</v>
+        <v>5.6266000975651043E-3</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" si="27"/>
-        <v>9.2041378557061737E-4</v>
+        <v>8.4799829354906264E-4</v>
       </c>
       <c r="N40" s="9">
         <f t="shared" si="27"/>
-        <v>1.693025022074468E-3</v>
+        <v>-2.5209404008838254E-3</v>
       </c>
       <c r="O40" s="9">
         <f t="shared" si="27"/>
-        <v>-4.397283432936494E-3</v>
+        <v>-1.2327354401073548E-2</v>
       </c>
       <c r="P40" s="9">
         <f t="shared" si="27"/>
-        <v>-8.327656798496258E-3</v>
+        <v>-1.6037863108084915E-2</v>
       </c>
       <c r="Q40" s="9">
         <f t="shared" si="27"/>
-        <v>-1.1497680539857447E-2</v>
+        <v>-1.7821888024283306E-2</v>
       </c>
       <c r="R40" s="9">
         <f t="shared" si="27"/>
-        <v>-1.9429938800258811E-2</v>
+        <v>-2.5945906293268151E-2</v>
       </c>
       <c r="S40" s="9">
         <f t="shared" si="27"/>
-        <v>-3.1145844619042212E-2</v>
+        <v>-3.7635011401500773E-2</v>
       </c>
       <c r="T40" s="9">
         <f t="shared" si="27"/>
-        <v>-3.0024558202549428E-2</v>
+        <v>-3.6946469901595363E-2</v>
       </c>
       <c r="U40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.8563994795707814E-2</v>
+        <v>-3.5931760463902257E-2</v>
       </c>
       <c r="V40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.8271320523535731E-2</v>
+        <v>-3.5990032219404944E-2</v>
       </c>
       <c r="W40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.7095634381200051E-2</v>
+        <v>-3.5208789967312942E-2</v>
       </c>
       <c r="X40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.5916753907988893E-2</v>
+        <v>-3.4431941950816308E-2</v>
       </c>
       <c r="Y40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.8566860573285113E-2</v>
+        <v>-3.7211305636182884E-2</v>
       </c>
       <c r="Z40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.6087270048228944E-2</v>
+        <v>-3.5089507176317036E-2</v>
       </c>
       <c r="AA40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.3603703989491576E-2</v>
+        <v>-3.2973717281252674E-2</v>
       </c>
       <c r="AB40" s="9">
         <f t="shared" si="27"/>
-        <v>-2.4613096859529143E-2</v>
+        <v>-3.4173320526103917E-2</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.45">
@@ -3696,103 +3696,103 @@
       </c>
       <c r="D41" s="9">
         <f t="shared" si="27"/>
-        <v>-1.1488105570833379E-3</v>
+        <v>3.761689971224641E-4</v>
       </c>
       <c r="E41" s="9">
         <f t="shared" si="27"/>
-        <v>2.3579216513605339E-2</v>
+        <v>2.5128054135710953E-2</v>
       </c>
       <c r="F41" s="9">
         <f t="shared" si="27"/>
-        <v>2.3983951013414481E-2</v>
+        <v>2.5618890518502815E-2</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="27"/>
-        <v>2.0838698177904652E-2</v>
+        <v>2.2592515935600882E-2</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="27"/>
-        <v>1.8673144798441746E-2</v>
+        <v>2.0598262430275016E-2</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" si="27"/>
-        <v>-2.7169332527845799E-2</v>
+        <v>-4.7068030220635874E-2</v>
       </c>
       <c r="J41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.5189083530267035E-2</v>
+        <v>-5.2972538784857914E-2</v>
       </c>
       <c r="K41" s="9">
         <f t="shared" si="27"/>
-        <v>-4.3869965585274062E-2</v>
+        <v>-5.8364340662431721E-2</v>
       </c>
       <c r="L41" s="9">
         <f t="shared" si="27"/>
-        <v>-5.0266382155730004E-2</v>
+        <v>-6.0874285389132705E-2</v>
       </c>
       <c r="M41" s="9">
         <f t="shared" si="27"/>
-        <v>-4.8102626965580292E-2</v>
+        <v>-5.4467763418119521E-2</v>
       </c>
       <c r="N41" s="9">
         <f t="shared" si="27"/>
-        <v>-5.2498937645696353E-2</v>
+        <v>-5.4148971003749789E-2</v>
       </c>
       <c r="O41" s="9">
         <f t="shared" si="27"/>
-        <v>-5.5643481728694884E-2</v>
+        <v>-5.2481625612405818E-2</v>
       </c>
       <c r="P41" s="9">
         <f t="shared" si="27"/>
-        <v>-4.8812517809093306E-2</v>
+        <v>-4.1225595550102204E-2</v>
       </c>
       <c r="Q41" s="9">
         <f t="shared" si="27"/>
-        <v>-5.2154186835020461E-2</v>
+        <v>-4.0874650423332735E-2</v>
       </c>
       <c r="R41" s="9">
         <f t="shared" si="27"/>
-        <v>-5.3306301489592166E-2</v>
+        <v>-3.8699782857193034E-2</v>
       </c>
       <c r="S41" s="9">
         <f t="shared" si="27"/>
-        <v>-4.2385598460603129E-2</v>
+        <v>-2.6696702822214938E-2</v>
       </c>
       <c r="T41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.977881330479642E-2</v>
+        <v>-2.2947065356931237E-2</v>
       </c>
       <c r="U41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.8497444709338455E-2</v>
+        <v>-2.0734019713675778E-2</v>
       </c>
       <c r="V41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.5959257605570644E-2</v>
+        <v>-1.7508413230223632E-2</v>
       </c>
       <c r="W41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.5349493009115163E-2</v>
+        <v>-1.6305110773965084E-2</v>
       </c>
       <c r="X41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.5531900152244084E-2</v>
+        <v>-1.5982812686560266E-2</v>
       </c>
       <c r="Y41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.2480175291361865E-2</v>
+        <v>-1.2612157837409224E-2</v>
       </c>
       <c r="Z41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.5001959198947108E-2</v>
+        <v>-1.4606406555096874E-2</v>
       </c>
       <c r="AA41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.7868740019912882E-2</v>
+        <v>-1.6943078329687999E-2</v>
       </c>
       <c r="AB41" s="9">
         <f t="shared" si="27"/>
-        <v>-3.7500221331121332E-2</v>
+        <v>-1.6214667107843223E-2</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.45">
@@ -3806,103 +3806,103 @@
       </c>
       <c r="D44" s="1">
         <f>D38*D$20</f>
-        <v>-305.25205173879328</v>
+        <v>-334.83817840545959</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" ref="E44:AB47" si="29">E38*E$20</f>
-        <v>-1290.6685304271091</v>
+        <v>-1508.0602125572545</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="29"/>
-        <v>-1295.5488199311433</v>
+        <v>-1702.3601565979204</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="29"/>
-        <v>-1280.3391832914449</v>
+        <v>-1883.2385411639214</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="29"/>
-        <v>-1280.0095879727057</v>
+        <v>-2083.5946788716201</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" si="29"/>
-        <v>19.469997496918342</v>
+        <v>-181.09799440439284</v>
       </c>
       <c r="J44" s="1">
         <f t="shared" si="29"/>
-        <v>173.29075047931366</v>
+        <v>164.87987924441418</v>
       </c>
       <c r="K44" s="1">
         <f t="shared" si="29"/>
-        <v>336.23240247813078</v>
+        <v>477.57319726540646</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="29"/>
-        <v>576.10037838286576</v>
+        <v>841.96043431462624</v>
       </c>
       <c r="M44" s="1">
         <f t="shared" si="29"/>
-        <v>527.38343837468108</v>
+        <v>877.58663873862474</v>
       </c>
       <c r="N44" s="1">
         <f t="shared" si="29"/>
-        <v>607.7206910222427</v>
+        <v>1022.8576988676289</v>
       </c>
       <c r="O44" s="1">
         <f t="shared" si="29"/>
-        <v>826.99709829967014</v>
+        <v>1287.1296477197495</v>
       </c>
       <c r="P44" s="1">
         <f t="shared" si="29"/>
-        <v>730.06826009887982</v>
+        <v>1123.6367035279909</v>
       </c>
       <c r="Q44" s="1">
         <f t="shared" si="29"/>
-        <v>924.14561633273377</v>
+        <v>1199.0307955276985</v>
       </c>
       <c r="R44" s="1">
         <f t="shared" si="29"/>
-        <v>1311.7374737909886</v>
+        <v>1414.3168851620621</v>
       </c>
       <c r="S44" s="1">
         <f t="shared" si="29"/>
-        <v>1466.9351584684923</v>
+        <v>1442.299053251118</v>
       </c>
       <c r="T44" s="1">
         <f t="shared" si="29"/>
-        <v>1256.6433972607281</v>
+        <v>1192.1030396317954</v>
       </c>
       <c r="U44" s="1">
         <f t="shared" si="29"/>
-        <v>1086.7975510161525</v>
+        <v>991.55471606959054</v>
       </c>
       <c r="V44" s="1">
         <f t="shared" si="29"/>
-        <v>913.14465633065072</v>
+        <v>792.29868013301609</v>
       </c>
       <c r="W44" s="1">
         <f t="shared" si="29"/>
-        <v>782.44082819164294</v>
+        <v>642.03761577796854</v>
       </c>
       <c r="X44" s="1">
         <f t="shared" si="29"/>
-        <v>684.1038890532493</v>
+        <v>528.52425176991881</v>
       </c>
       <c r="Y44" s="1">
         <f t="shared" si="29"/>
-        <v>610.13618388425641</v>
+        <v>446.87603037254871</v>
       </c>
       <c r="Z44" s="1">
         <f t="shared" si="29"/>
-        <v>554.38491420581329</v>
+        <v>387.27705304928395</v>
       </c>
       <c r="AA44" s="1">
         <f t="shared" si="29"/>
-        <v>512.52474273252369</v>
+        <v>342.20974736001591</v>
       </c>
       <c r="AB44" s="1">
         <f t="shared" si="29"/>
-        <v>481.12313390038395</v>
+        <v>307.70993134918473</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.45">
@@ -3911,103 +3911,103 @@
       </c>
       <c r="D45" s="1">
         <f t="shared" ref="D45:S47" si="30">D39*D$20</f>
-        <v>307.47246430364589</v>
+        <v>290.69966430364622</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="30"/>
-        <v>423.45645071446546</v>
+        <v>461.31243108779756</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="30"/>
-        <v>512.82046363371285</v>
+        <v>608.65666193705215</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="30"/>
-        <v>567.79643404502849</v>
+        <v>723.92612192014428</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="30"/>
-        <v>608.61517031097185</v>
+        <v>824.7104679507313</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" si="30"/>
-        <v>676.14917775389688</v>
+        <v>956.81186933991808</v>
       </c>
       <c r="J45" s="1">
         <f t="shared" si="30"/>
-        <v>770.72880768949767</v>
+        <v>969.30741863726735</v>
       </c>
       <c r="K45" s="1">
         <f t="shared" si="30"/>
-        <v>883.26189108145263</v>
+        <v>996.81227815554894</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="30"/>
-        <v>1042.1618920705926</v>
+        <v>1071.6478864186265</v>
       </c>
       <c r="M45" s="1">
         <f t="shared" si="30"/>
-        <v>1112.9821344688801</v>
+        <v>1052.0433240164293</v>
       </c>
       <c r="N45" s="1">
         <f t="shared" si="30"/>
-        <v>1232.5971922407552</v>
+        <v>1079.6994275817103</v>
       </c>
       <c r="O45" s="1">
         <f t="shared" si="30"/>
-        <v>1417.4526068655739</v>
+        <v>1169.5572394491458</v>
       </c>
       <c r="P45" s="1">
         <f t="shared" si="30"/>
-        <v>1502.4476129502546</v>
+        <v>1133.5212196829389</v>
       </c>
       <c r="Q45" s="1">
         <f t="shared" si="30"/>
-        <v>1633.0517010963479</v>
+        <v>1179.5752796393569</v>
       </c>
       <c r="R45" s="1">
         <f t="shared" si="30"/>
-        <v>1638.5925971304387</v>
+        <v>1255.9546832043777</v>
       </c>
       <c r="S45" s="1">
         <f t="shared" si="30"/>
-        <v>1562.9473213237286</v>
+        <v>1281.6511818179683</v>
       </c>
       <c r="T45" s="1">
         <f t="shared" si="29"/>
-        <v>1618.6719649048985</v>
+        <v>1350.2769785549722</v>
       </c>
       <c r="U45" s="1">
         <f t="shared" si="29"/>
-        <v>1674.5935172094612</v>
+        <v>1419.8209223601418</v>
       </c>
       <c r="V45" s="1">
         <f t="shared" si="29"/>
-        <v>1730.6865915068852</v>
+        <v>1490.0334453316093</v>
       </c>
       <c r="W45" s="1">
         <f t="shared" si="29"/>
-        <v>1786.8963122550767</v>
+        <v>1561.1619970624345</v>
       </c>
       <c r="X45" s="1">
         <f t="shared" si="29"/>
-        <v>1843.2136193396275</v>
+        <v>1633.1100664493613</v>
       </c>
       <c r="Y45" s="1">
         <f t="shared" si="29"/>
-        <v>1899.6226431095167</v>
+        <v>1693.6984269051297</v>
       </c>
       <c r="Z45" s="1">
         <f t="shared" si="29"/>
-        <v>1956.0589543330473</v>
+        <v>1751.718449652283</v>
       </c>
       <c r="AA45" s="1">
         <f t="shared" si="29"/>
-        <v>2012.5838146170247</v>
+        <v>1810.2394894380616</v>
       </c>
       <c r="AB45" s="1">
         <f t="shared" si="29"/>
-        <v>2069.1905366804363</v>
+        <v>1869.1094684651996</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.45">
@@ -4016,103 +4016,103 @@
       </c>
       <c r="D46" s="1">
         <f t="shared" si="30"/>
-        <v>40.012319301135818</v>
+        <v>30.28847130113607</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="29"/>
-        <v>37.759431370393642</v>
+        <v>149.30412021990466</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="29"/>
-        <v>-25.089432557145251</v>
+        <v>204.9006959174211</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="29"/>
-        <v>42.380680418761138</v>
+        <v>399.11343155382173</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="29"/>
-        <v>98.534002127179548</v>
+        <v>586.48773833395694</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" si="29"/>
-        <v>93.205827795666949</v>
+        <v>704.45682036471442</v>
       </c>
       <c r="J46" s="1">
         <f t="shared" si="29"/>
-        <v>129.07914357579159</v>
+        <v>594.92298805325709</v>
       </c>
       <c r="K46" s="1">
         <f t="shared" si="29"/>
-        <v>179.82119690895362</v>
+        <v>495.89453728356131</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="29"/>
-        <v>45.384602991804975</v>
+        <v>194.88796150130312</v>
       </c>
       <c r="M46" s="1">
         <f t="shared" si="29"/>
-        <v>31.999666502722224</v>
+        <v>30.517159331002105</v>
       </c>
       <c r="N46" s="1">
         <f t="shared" si="29"/>
-        <v>61.325622630125707</v>
+        <v>-93.531489177499338</v>
       </c>
       <c r="O46" s="1">
         <f t="shared" si="29"/>
-        <v>-164.37967567557567</v>
+        <v>-467.28786511224808</v>
       </c>
       <c r="P46" s="1">
         <f t="shared" si="29"/>
-        <v>-325.36872901818276</v>
+        <v>-632.16561894852521</v>
       </c>
       <c r="Q46" s="1">
         <f t="shared" si="29"/>
-        <v>-461.91634347532607</v>
+        <v>-722.21041047147094</v>
       </c>
       <c r="R46" s="1">
         <f t="shared" si="29"/>
-        <v>-788.11789680261052</v>
+        <v>-1071.7283209582699</v>
       </c>
       <c r="S46" s="1">
         <f t="shared" si="29"/>
-        <v>-1283.3727311369637</v>
+        <v>-1593.5514759865277</v>
       </c>
       <c r="T46" s="1">
         <f t="shared" si="29"/>
-        <v>-1236.7607979070376</v>
+        <v>-1568.3156189545955</v>
       </c>
       <c r="U46" s="1">
         <f t="shared" si="29"/>
-        <v>-1176.1805395748368</v>
+        <v>-1529.0528350094241</v>
       </c>
       <c r="V46" s="1">
         <f t="shared" si="29"/>
-        <v>-1163.6918551085487</v>
+        <v>-1535.3942724970357</v>
       </c>
       <c r="W46" s="1">
         <f t="shared" si="29"/>
-        <v>-1114.8639240406073</v>
+        <v>-1505.8458262393735</v>
       </c>
       <c r="X46" s="1">
         <f t="shared" si="29"/>
-        <v>-1065.9284066363075</v>
+        <v>-1476.33897852273</v>
       </c>
       <c r="Y46" s="1">
         <f t="shared" si="29"/>
-        <v>-1174.437537676135</v>
+        <v>-1598.7160428737477</v>
       </c>
       <c r="Z46" s="1">
         <f t="shared" si="29"/>
-        <v>-1072.0486728439348</v>
+        <v>-1510.3112591470854</v>
       </c>
       <c r="AA46" s="1">
         <f t="shared" si="29"/>
-        <v>-969.57125895128888</v>
+        <v>-1421.8511370323611</v>
       </c>
       <c r="AB46" s="1">
         <f t="shared" si="29"/>
-        <v>-1010.5903085634122</v>
+        <v>-1476.3270090822439</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.45">
@@ -4121,103 +4121,103 @@
       </c>
       <c r="D47" s="1">
         <f t="shared" si="30"/>
-        <v>-42.232731865991006</v>
+        <v>13.850042800675759</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="29"/>
-        <v>829.45264834224895</v>
+        <v>897.44366124955332</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="29"/>
-        <v>807.81778885457993</v>
+        <v>888.80279874344774</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="29"/>
-        <v>670.16206882765789</v>
+        <v>760.19898768995813</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="29"/>
-        <v>572.8604155345522</v>
+        <v>672.39647258693026</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="29"/>
-        <v>-788.82500304647931</v>
+        <v>-1480.1706953002404</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="29"/>
-        <v>-1073.0987017446039</v>
+        <v>-1729.1102859349405</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="29"/>
-        <v>-1399.3154904685371</v>
+        <v>-1970.2800127045134</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="29"/>
-        <v>-1663.6468734452594</v>
+        <v>-2108.4962822345597</v>
       </c>
       <c r="M47" s="1">
         <f t="shared" si="29"/>
-        <v>-1672.3652393462814</v>
+        <v>-1960.1471220860556</v>
       </c>
       <c r="N47" s="1">
         <f t="shared" si="29"/>
-        <v>-1901.6435058931238</v>
+        <v>-2009.0256372718377</v>
       </c>
       <c r="O47" s="1">
         <f t="shared" si="29"/>
-        <v>-2080.0700294896778</v>
+        <v>-1989.3990220566448</v>
       </c>
       <c r="P47" s="1">
         <f t="shared" si="29"/>
-        <v>-1907.1471440309545</v>
+        <v>-1624.9923042624052</v>
       </c>
       <c r="Q47" s="1">
         <f t="shared" si="29"/>
-        <v>-2095.2809739537547</v>
+        <v>-1656.3956646955842</v>
       </c>
       <c r="R47" s="1">
         <f t="shared" si="29"/>
-        <v>-2162.2121741188212</v>
+        <v>-1598.543247408177</v>
       </c>
       <c r="S47" s="1">
         <f t="shared" si="29"/>
-        <v>-1746.5097486552513</v>
+        <v>-1130.3987590825559</v>
       </c>
       <c r="T47" s="1">
         <f t="shared" si="29"/>
-        <v>-1638.5545642585919</v>
+        <v>-974.06439923217624</v>
       </c>
       <c r="U47" s="1">
         <f t="shared" si="29"/>
-        <v>-1585.210528650781</v>
+        <v>-882.32280342030822</v>
       </c>
       <c r="V47" s="1">
         <f t="shared" si="29"/>
-        <v>-1480.139392728986</v>
+        <v>-746.93785296758915</v>
       </c>
       <c r="W47" s="1">
         <f t="shared" si="29"/>
-        <v>-1454.4732164061147</v>
+        <v>-697.35378660102788</v>
       </c>
       <c r="X47" s="1">
         <f t="shared" si="29"/>
-        <v>-1461.3891017565679</v>
+        <v>-685.29533969654892</v>
       </c>
       <c r="Y47" s="1">
         <f t="shared" si="29"/>
-        <v>-1335.3212893176376</v>
+        <v>-541.85841440392778</v>
       </c>
       <c r="Z47" s="1">
         <f t="shared" si="29"/>
-        <v>-1438.3951956949315</v>
+        <v>-628.68424355448644</v>
       </c>
       <c r="AA47" s="1">
         <f t="shared" si="29"/>
-        <v>-1555.5372983982613</v>
+        <v>-730.59809976571864</v>
       </c>
       <c r="AB47" s="1">
         <f t="shared" si="29"/>
-        <v>-1539.7233620174015</v>
+        <v>-700.49239073214517</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.45">
@@ -4317,83 +4317,83 @@
       </c>
       <c r="I52" s="1">
         <f>-H44</f>
-        <v>1280.0095879727057</v>
+        <v>2083.5946788716201</v>
       </c>
       <c r="J52" s="1">
         <f t="shared" ref="J52:AB52" si="31">-0.25*I44</f>
-        <v>-4.8674993742295856</v>
+        <v>45.274498601098209</v>
       </c>
       <c r="K52" s="1">
         <f t="shared" si="31"/>
-        <v>-43.322687619828415</v>
+        <v>-41.219969811103546</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" si="31"/>
-        <v>-84.058100619532695</v>
+        <v>-119.39329931635162</v>
       </c>
       <c r="M52" s="1">
         <f t="shared" si="31"/>
-        <v>-144.02509459571644</v>
+        <v>-210.49010857865656</v>
       </c>
       <c r="N52" s="1">
         <f t="shared" si="31"/>
-        <v>-131.84585959367027</v>
+        <v>-219.39665968465619</v>
       </c>
       <c r="O52" s="1">
         <f t="shared" si="31"/>
-        <v>-151.93017275556068</v>
+        <v>-255.71442471690722</v>
       </c>
       <c r="P52" s="1">
         <f t="shared" si="31"/>
-        <v>-206.74927457491754</v>
+        <v>-321.78241192993738</v>
       </c>
       <c r="Q52" s="1">
         <f t="shared" si="31"/>
-        <v>-182.51706502471995</v>
+        <v>-280.90917588199773</v>
       </c>
       <c r="R52" s="1">
         <f t="shared" si="31"/>
-        <v>-231.03640408318344</v>
+        <v>-299.75769888192463</v>
       </c>
       <c r="S52" s="1">
         <f t="shared" si="31"/>
-        <v>-327.93436844774715</v>
+        <v>-353.57922129051553</v>
       </c>
       <c r="T52" s="1">
         <f t="shared" si="31"/>
-        <v>-366.73378961712308</v>
+        <v>-360.57476331277951</v>
       </c>
       <c r="U52" s="1">
         <f t="shared" si="31"/>
-        <v>-314.16084931518202</v>
+        <v>-298.02575990794884</v>
       </c>
       <c r="V52" s="1">
         <f t="shared" si="31"/>
-        <v>-271.69938775403813</v>
+        <v>-247.88867901739764</v>
       </c>
       <c r="W52" s="1">
         <f t="shared" si="31"/>
-        <v>-228.28616408266268</v>
+        <v>-198.07467003325402</v>
       </c>
       <c r="X52" s="1">
         <f t="shared" si="31"/>
-        <v>-195.61020704791073</v>
+        <v>-160.50940394449213</v>
       </c>
       <c r="Y52" s="1">
         <f t="shared" si="31"/>
-        <v>-171.02597226331233</v>
+        <v>-132.1310629424797</v>
       </c>
       <c r="Z52" s="1">
         <f t="shared" si="31"/>
-        <v>-152.5340459710641</v>
+        <v>-111.71900759313718</v>
       </c>
       <c r="AA52" s="1">
         <f t="shared" si="31"/>
-        <v>-138.59622855145332</v>
+        <v>-96.819263262320987</v>
       </c>
       <c r="AB52" s="1">
         <f t="shared" si="31"/>
-        <v>-128.13118568313092</v>
+        <v>-85.552436840003978</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.45">
@@ -4405,103 +4405,103 @@
       </c>
       <c r="D53">
         <f>$C53*D60</f>
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="E53">
         <f t="shared" ref="E53:AB53" si="32">$C53*E60</f>
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="F53">
         <f t="shared" si="32"/>
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="G53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="H53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="I53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="J53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="K53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="L53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="M53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="N53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="O53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="P53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="Q53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="R53">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>-12</v>
       </c>
       <c r="S53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="T53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="U53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="V53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="W53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="X53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="Y53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="Z53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="AA53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="AB53">
         <f t="shared" si="32"/>
-        <v>53</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.45">
@@ -4618,103 +4618,103 @@
       </c>
       <c r="D55" s="1">
         <f>-SUM(D52:D54)</f>
-        <v>-200.31065485156577</v>
+        <v>-138.31065485156577</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" ref="E55:AB55" si="34">-SUM(E52:E54)</f>
-        <v>799.6893451484342</v>
+        <v>861.6893451484342</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="34"/>
-        <v>-84.625854897576062</v>
+        <v>-22.625854897576062</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="34"/>
-        <v>-202.24716460070755</v>
+        <v>-144.24716460070755</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" si="34"/>
-        <v>-156.30299823488613</v>
+        <v>-98.302998234886132</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="34"/>
-        <v>-1436.3125862075919</v>
+        <v>-2181.8976771065063</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="34"/>
-        <v>-35.480575825296057</v>
+        <v>-27.62257380062384</v>
       </c>
       <c r="K55" s="1">
         <f t="shared" si="34"/>
-        <v>-84.151068281446797</v>
+        <v>-28.253786090171666</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="34"/>
-        <v>-43.415655281742517</v>
+        <v>49.919543415076404</v>
       </c>
       <c r="M55" s="1">
         <f t="shared" si="34"/>
-        <v>259.82814566903426</v>
+        <v>384.29315965197441</v>
       </c>
       <c r="N55" s="1">
         <f t="shared" si="34"/>
-        <v>16.272149741199513</v>
+        <v>161.82294983218543</v>
       </c>
       <c r="O55" s="1">
         <f t="shared" si="34"/>
-        <v>36.35646290308992</v>
+        <v>198.14071486443646</v>
       </c>
       <c r="P55" s="1">
         <f t="shared" si="34"/>
-        <v>440.80320925392834</v>
+        <v>613.83634660894813</v>
       </c>
       <c r="Q55" s="1">
         <f t="shared" si="34"/>
-        <v>19.146259114577589</v>
+        <v>175.53836997185536</v>
       </c>
       <c r="R55" s="1">
         <f t="shared" si="34"/>
-        <v>67.665598173041076</v>
+        <v>231.38689297178226</v>
       </c>
       <c r="S55" s="1">
         <f t="shared" si="34"/>
-        <v>575.87021108857755</v>
+        <v>666.51506393134594</v>
       </c>
       <c r="T55" s="1">
         <f t="shared" si="34"/>
-        <v>201.15289668885669</v>
+        <v>259.99387038451312</v>
       </c>
       <c r="U55" s="1">
         <f t="shared" si="34"/>
-        <v>148.57995638691563</v>
+        <v>197.44486697968244</v>
       </c>
       <c r="V55" s="1">
         <f t="shared" si="34"/>
-        <v>209.30377758517542</v>
+        <v>250.49306884853493</v>
       </c>
       <c r="W55" s="1">
         <f t="shared" si="34"/>
-        <v>129.6679537629129</v>
+        <v>164.45645971350424</v>
       </c>
       <c r="X55" s="1">
         <f t="shared" si="34"/>
-        <v>96.991996728160956</v>
+        <v>126.89119362474236</v>
       </c>
       <c r="Y55" s="1">
         <f t="shared" si="34"/>
-        <v>229.94412707302922</v>
+        <v>256.04921775219657</v>
       </c>
       <c r="Z55" s="1">
         <f t="shared" si="34"/>
-        <v>0.5814923623947692</v>
+        <v>24.766453984467844</v>
       </c>
       <c r="AA55" s="1">
         <f t="shared" si="34"/>
-        <v>-13.356325057216011</v>
+        <v>9.8667096536516539</v>
       </c>
       <c r="AB55" s="1">
         <f t="shared" si="34"/>
-        <v>119.75695735866562</v>
+        <v>142.17820851553867</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.45">
@@ -4727,79 +4727,79 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="E60">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="F60">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="G60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="H60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="I60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="J60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="K60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="L60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="M60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="N60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="O60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="P60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="Q60">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="R60">
-        <v>83</v>
+        <v>-12</v>
       </c>
       <c r="S60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="T60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="U60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="V60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="W60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="X60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="Y60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="Z60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="AA60">
-        <v>53</v>
+        <v>-12</v>
       </c>
       <c r="AB60">
-        <v>53</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="14.65" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -4992,79 +4992,79 @@
         <v>21</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="L65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="M65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="N65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="O65">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="P65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="T65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="U65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="V65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="W65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Z65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AA65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB65">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.45">

</xml_diff>